<commit_message>
added AVERAGES in excel
</commit_message>
<xml_diff>
--- a/BILANCIA DI COLUMB/bilancia di columb dati.xlsx
+++ b/BILANCIA DI COLUMB/bilancia di columb dati.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t xml:space="preserve">diametro sfere</t>
   </si>
@@ -43,6 +43,9 @@
     <t>teta3</t>
   </si>
   <si>
+    <t>AVERAGE</t>
+  </si>
+  <si>
     <t>V</t>
   </si>
   <si>
@@ -62,6 +65,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="160" formatCode="0.0"/>
+  </numFmts>
   <fonts count="1">
     <font>
       <sz val="11.000000"/>
@@ -90,11 +96,12 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="2" xfId="0" applyNumberFormat="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="1" xfId="0" applyNumberFormat="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="160" xfId="0" applyNumberFormat="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
       <protection hidden="0" locked="1"/>
     </xf>
@@ -661,6 +668,9 @@
       <c r="D1" t="s">
         <v>7</v>
       </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="2" ht="14.25">
       <c r="A2" s="1">
@@ -675,7 +685,10 @@
       <c r="D2">
         <v>186</v>
       </c>
-      <c r="E2" s="2"/>
+      <c r="E2" s="2">
+        <f>AVERAGE(B2:D2)</f>
+        <v>186.33333333333334</v>
+      </c>
     </row>
     <row r="3" ht="14.25">
       <c r="A3" s="1">
@@ -690,7 +703,10 @@
       <c r="D3" s="3">
         <v>126</v>
       </c>
-      <c r="E3" s="2"/>
+      <c r="E3" s="2">
+        <f>AVERAGE(B3:D3)</f>
+        <v>124.66666666666667</v>
+      </c>
     </row>
     <row r="4" ht="14.25">
       <c r="A4" s="1">
@@ -705,7 +721,10 @@
       <c r="D4" s="3">
         <v>103</v>
       </c>
-      <c r="E4" s="2"/>
+      <c r="E4" s="2">
+        <f>AVERAGE(B4:D4)</f>
+        <v>105.33333333333333</v>
+      </c>
     </row>
     <row r="5" ht="14.25">
       <c r="A5" s="1">
@@ -720,7 +739,10 @@
       <c r="D5">
         <v>90</v>
       </c>
-      <c r="E5" s="2"/>
+      <c r="E5" s="2">
+        <f>AVERAGE(B5:D5)</f>
+        <v>92.333333333333329</v>
+      </c>
     </row>
     <row r="6" ht="14.25">
       <c r="A6" s="1">
@@ -735,7 +757,10 @@
       <c r="D6">
         <v>51</v>
       </c>
-      <c r="E6" s="2"/>
+      <c r="E6" s="2">
+        <f>AVERAGE(B6:D6)</f>
+        <v>52</v>
+      </c>
     </row>
     <row r="7" ht="14.25">
       <c r="A7" s="1">
@@ -750,7 +775,10 @@
       <c r="D7">
         <v>31</v>
       </c>
-      <c r="E7" s="2"/>
+      <c r="E7" s="2">
+        <f>AVERAGE(B7:D7)</f>
+        <v>32.333333333333336</v>
+      </c>
     </row>
     <row r="8" ht="14.25">
       <c r="A8" s="1">
@@ -765,7 +793,10 @@
       <c r="D8">
         <v>18</v>
       </c>
-      <c r="E8" s="2"/>
+      <c r="E8" s="2">
+        <f>AVERAGE(B8:D8)</f>
+        <v>18</v>
+      </c>
     </row>
     <row r="9" ht="14.25">
       <c r="A9" s="1"/>
@@ -949,7 +980,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s">
         <v>5</v>
@@ -959,6 +990,9 @@
       </c>
       <c r="D1" t="s">
         <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="2">
@@ -974,6 +1008,10 @@
       <c r="D2">
         <v>6</v>
       </c>
+      <c r="E2" s="4">
+        <f>AVERAGE(B2:D2)</f>
+        <v>7</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3">
@@ -988,6 +1026,10 @@
       <c r="D3">
         <v>17</v>
       </c>
+      <c r="E3" s="4">
+        <f>AVERAGE(B3:D3)</f>
+        <v>16</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4">
@@ -1002,6 +1044,10 @@
       <c r="D4">
         <v>34</v>
       </c>
+      <c r="E4" s="4">
+        <f>AVERAGE(B4:D4)</f>
+        <v>33.666666666666664</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5">
@@ -1016,6 +1062,10 @@
       <c r="D5">
         <v>48</v>
       </c>
+      <c r="E5" s="4">
+        <f>AVERAGE(B5:D5)</f>
+        <v>48.666666666666664</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -1029,6 +1079,10 @@
       </c>
       <c r="D6">
         <v>73</v>
+      </c>
+      <c r="E6" s="4">
+        <f>AVERAGE(B6:D6)</f>
+        <v>71.666666666666671</v>
       </c>
     </row>
     <row r="7"/>
@@ -1051,7 +1105,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
         <v>5</v>
@@ -1061,6 +1115,9 @@
       </c>
       <c r="D1" t="s">
         <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="2">
@@ -1076,6 +1133,10 @@
       <c r="D2">
         <v>23</v>
       </c>
+      <c r="E2" s="4">
+        <f>AVERAGE(B2:D2)</f>
+        <v>21.333333333333332</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3">
@@ -1090,6 +1151,10 @@
       <c r="D3">
         <v>36</v>
       </c>
+      <c r="E3" s="4">
+        <f>AVERAGE(B3:D3)</f>
+        <v>38</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4">
@@ -1104,6 +1169,10 @@
       <c r="D4">
         <v>53</v>
       </c>
+      <c r="E4" s="4">
+        <f>AVERAGE(B4:D4)</f>
+        <v>52</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5">
@@ -1118,19 +1187,27 @@
       <c r="D5">
         <v>59</v>
       </c>
+      <c r="E5" s="4">
+        <f>AVERAGE(B5:D5)</f>
+        <v>60</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
         <v>6</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="5">
         <v>70</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="5">
         <v>72</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="5">
         <v>73</v>
+      </c>
+      <c r="E6" s="4">
+        <f>AVERAGE(B6:D6)</f>
+        <v>71.666666666666671</v>
       </c>
     </row>
   </sheetData>
@@ -1152,7 +1229,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
         <v>5</v>
@@ -1164,10 +1241,10 @@
         <v>7</v>
       </c>
       <c r="E1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2">

</xml_diff>